<commit_message>
Remove user management card and clean up development tools
- Removed Gebruikersbeheer card from settings dashboard (obsolete without authentication)
- Deleted 14 development/testing scripts from tools/ folder:
  - API testing scripts (_check_api, _call_local_client, _list_routes)
  - Debug utilities (_read_excel_headers, inspect_excel, inspect_zip_digipoort)
  - Comparison tools (compare_xmls, full_diff, parse_extracted_xml)
  - Test scripts (run_upload_test_digipoort, preview_normalize)
  - Build utilities (fetch_xsd, packagereport, sample_input.json)
- Kept only core functionality: generate_from_excel, minimal_xml_generator, tag_datasets
</commit_message>
<xml_diff>
--- a/docs/Input XML electr ziekmeldinge.xlsx
+++ b/docs/Input XML electr ziekmeldinge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hwa033\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZW\XML-automation-clean\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501AA98C-8948-4519-BC11-16C5D2204F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86559D07-3AB9-420B-A7FC-A777F2A98434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7FE783C2-E503-42B3-B80D-538F4F9D880C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11235" xr2:uid="{7FE783C2-E503-42B3-B80D-538F4F9D880C}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
@@ -343,7 +343,7 @@
   <cellStyles count="3">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -27264,7 +27264,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -27583,26 +27583,26 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1796875" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -27640,7 +27640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>555501759</v>
       </c>
@@ -27680,7 +27680,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>555501760</v>
       </c>
@@ -27720,7 +27720,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
         <f>_xlfn.XLOOKUP(A4,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -27751,7 +27751,7 @@
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="13">
         <f>_xlfn.XLOOKUP(A5,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -27782,7 +27782,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <f>_xlfn.XLOOKUP(A6,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -27813,7 +27813,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <f>_xlfn.XLOOKUP(A7,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -27844,7 +27844,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <f>_xlfn.XLOOKUP(A8,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -27875,7 +27875,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <f>_xlfn.XLOOKUP(A9,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -27906,7 +27906,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <f>_xlfn.XLOOKUP(A10,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -27937,7 +27937,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="13">
         <f>_xlfn.XLOOKUP(A11,[1]NatuurlijkPersoon!$B:$B,[1]NatuurlijkPersoon!$G:$G)</f>
         <v>0</v>
@@ -28006,24 +28006,24 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -28061,7 +28061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -28102,7 +28102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -28132,7 +28132,7 @@
       </c>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -28165,29 +28165,29 @@
       <selection activeCell="A16" sqref="A16:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.08984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>31</v>
       </c>
@@ -28196,7 +28196,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>32</v>
       </c>
@@ -28206,7 +28206,7 @@
       <c r="C6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>33</v>
       </c>
@@ -28216,7 +28216,7 @@
       <c r="C7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>34</v>
       </c>
@@ -28226,7 +28226,7 @@
       <c r="C8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>35</v>
       </c>
@@ -28236,7 +28236,7 @@
       <c r="C9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>36</v>
       </c>
@@ -28246,7 +28246,7 @@
       <c r="C10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
@@ -28256,7 +28256,7 @@
       <c r="C11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>38</v>
       </c>
@@ -28266,7 +28266,7 @@
       <c r="C12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>39</v>
       </c>
@@ -28276,13 +28276,13 @@
       <c r="C13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
@@ -28291,7 +28291,7 @@
       </c>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>32</v>
       </c>
@@ -28300,7 +28300,7 @@
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>33</v>
       </c>
@@ -28309,7 +28309,7 @@
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>34</v>
       </c>
@@ -28318,7 +28318,7 @@
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>35</v>
       </c>
@@ -28327,7 +28327,7 @@
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>36</v>
       </c>
@@ -28336,7 +28336,7 @@
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>37</v>
       </c>
@@ -28345,7 +28345,7 @@
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>38</v>
       </c>
@@ -28354,7 +28354,7 @@
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>39</v>
       </c>

</xml_diff>